<commit_message>
use latest legacy import format of gbsl
</commit_message>
<xml_diff>
--- a/i18n/fr/docusaurus-plugin-content-docs/current/02-events/assets/[2024-05-21] Import-Format-GBSL.xlsx
+++ b/i18n/fr/docusaurus-plugin-content-docs/current/02-events/assets/[2024-05-21] Import-Format-GBSL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bauz\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{483B68CD-7227-4390-A935-FB494C44CC1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DBDF5F1-E068-44AD-860D-CA20C20B5A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{CD9F5FCB-EE8A-45FB-A0E3-6B2817874D8E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>KW</t>
   </si>
@@ -65,9 +65,6 @@
     <t>betroffene Lehrkräfte</t>
   </si>
   <si>
-    <t>Kategorie</t>
-  </si>
-  <si>
     <t>Beschreibung</t>
   </si>
   <si>
@@ -110,10 +107,10 @@
     <t>moe</t>
   </si>
   <si>
-    <t>Kategorie2</t>
-  </si>
-  <si>
-    <t>Kategorie3</t>
+    <t>GYM</t>
+  </si>
+  <si>
+    <t>WMS</t>
   </si>
 </sst>
 </file>
@@ -212,9 +209,9 @@
     <tableColumn id="7" xr3:uid="{428B1973-F349-48E1-804D-3A27E167F4FB}" name="Zeit Ende"/>
     <tableColumn id="8" xr3:uid="{A53DF7F0-FD33-47F9-8A6A-00310319FD70}" name="Ort"/>
     <tableColumn id="9" xr3:uid="{62F3EB51-186E-4D1A-A586-5368327DC2D0}" name="betroffene Lehrkräfte"/>
-    <tableColumn id="10" xr3:uid="{EF2BED3D-2652-46EB-A5F6-CC600FB220E7}" name="Kategorie"/>
-    <tableColumn id="11" xr3:uid="{5EA2DF2C-F35D-43EA-975E-BE41997E0183}" name="Kategorie2"/>
-    <tableColumn id="12" xr3:uid="{421BCC1B-C972-413B-B976-DB598193017E}" name="Kategorie3"/>
+    <tableColumn id="10" xr3:uid="{EF2BED3D-2652-46EB-A5F6-CC600FB220E7}" name="GYM"/>
+    <tableColumn id="11" xr3:uid="{5EA2DF2C-F35D-43EA-975E-BE41997E0183}" name="FMS"/>
+    <tableColumn id="12" xr3:uid="{421BCC1B-C972-413B-B976-DB598193017E}" name="WMS"/>
     <tableColumn id="13" xr3:uid="{7B20C2BE-DA8D-4213-8817-500AFE7DBAA6}" name="Beschreibung"/>
     <tableColumn id="14" xr3:uid="{974F373A-F4F5-481E-8818-6F417355A03D}" name="Jahrgangsstufe"/>
     <tableColumn id="15" xr3:uid="{50333CBA-2976-4FE2-8ADA-0A9BB56C95BB}" name="einzelne Klassen"/>
@@ -546,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BFB9E6A-F96B-4367-A0F9-2398CD2E8F2E}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -597,34 +594,34 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.35">
@@ -632,10 +629,10 @@
         <v>32</v>
       </c>
       <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
         <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
       </c>
       <c r="D2" s="1">
         <v>45509</v>
@@ -644,13 +641,13 @@
         <v>45527</v>
       </c>
       <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
         <v>19</v>
       </c>
-      <c r="K2" t="s">
+      <c r="O2" t="s">
         <v>20</v>
-      </c>
-      <c r="O2" t="s">
-        <v>21</v>
       </c>
       <c r="P2">
         <v>2</v>
@@ -659,10 +656,10 @@
         <v>2</v>
       </c>
       <c r="R2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S2" t="s">
         <v>22</v>
-      </c>
-      <c r="S2" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>